<commit_message>
updated the test projects
</commit_message>
<xml_diff>
--- a/raw/IFCB_dashboard_projects_list.xlsx
+++ b/raw/IFCB_dashboard_projects_list.xlsx
@@ -259,7 +259,7 @@
     <t>2022-11-15T13:46:07Z</t>
   </si>
   <si>
-    <t>2022-11-16T13:50:08Z</t>
+    <t>2022-11-16T20:26:44Z</t>
   </si>
   <si>
     <t>2022-10-18T19:32:40Z</t>
@@ -274,7 +274,7 @@
     <t>2022-11-12T16:31:24Z</t>
   </si>
   <si>
-    <t>2022-11-15T19:28:45Z</t>
+    <t>2022-11-16T20:46:22Z</t>
   </si>
   <si>
     <t>2022-11-10T10:54:16Z</t>
@@ -298,7 +298,7 @@
     <t>2019-03-20T20:53:33Z</t>
   </si>
   <si>
-    <t>2022-11-15T22:56:50Z</t>
+    <t>2022-11-16T17:47:53Z</t>
   </si>
   <si>
     <t>2018-04-12T02:11:17Z</t>
@@ -825,7 +825,7 @@
         <v>78</v>
       </c>
       <c r="K3" t="s">
-        <v>112</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -985,7 +985,7 @@
         <v>83</v>
       </c>
       <c r="K8" t="s">
-        <v>76</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1273,7 +1273,7 @@
         <v>92</v>
       </c>
       <c r="K17" t="s">
-        <v>112</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1465,7 +1465,7 @@
         <v>98</v>
       </c>
       <c r="K23" t="s">
-        <v>76</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:11">

</xml_diff>